<commit_message>
Add file for week2
</commit_message>
<xml_diff>
--- a/Week 1/Steps.xlsx
+++ b/Week 1/Steps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Code\School\Jaar 2\Semester 4\AS-AP4-Jeffrey van den Elshout\Synchronisation\Week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Code\School\Jaar 2\Semester 4\Synchronization\Week 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64F6856E-49C4-4AFC-92AF-D32427190149}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2A7E57-974E-4126-B61B-9C10CC841563}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34245" yWindow="10350" windowWidth="25425" windowHeight="17280" xr2:uid="{1E8C350D-24A7-4665-8C8E-37350E5BC664}"/>
+    <workbookView xWindow="42420" yWindow="6645" windowWidth="25425" windowHeight="17280" xr2:uid="{1E8C350D-24A7-4665-8C8E-37350E5BC664}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="9">
   <si>
     <t>flag[0]</t>
   </si>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEBE55A-1052-4000-B59A-3114D1B613A6}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:P8"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,6 +714,166 @@
         <v>7</v>
       </c>
     </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>